<commit_message>
Created the schematic with new ios.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/VestibularH2_BOM.xlsx
+++ b/Hardware/PCB/VestibularH2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Palma\Documents\GitHub\Neurogears\device.vestibularH2\Hardware\PCB\VestibularVR H2-module v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\open-ephys\device.vestibularH2\Hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837F4358-DEA1-414B-B967-E1AD06CEA578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E8F49C-C7C6-40B2-9971-F856DA0B613A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VestibularVR H2-module v1.1" sheetId="25" r:id="rId1"/>
@@ -512,9 +512,6 @@
     <t>OEPS070020</t>
   </si>
   <si>
-    <t>X4</t>
-  </si>
-  <si>
     <t>X6</t>
   </si>
   <si>
@@ -554,18 +551,9 @@
     <t>OEPS070025</t>
   </si>
   <si>
-    <t>C1, C3, C5, C7, C9, C12, C14, C16, C17, C18, C25, C26, C27, C28, C29</t>
-  </si>
-  <si>
-    <t>R2, R6, R8, R12, R13, R17, R18, R19, R34</t>
-  </si>
-  <si>
     <t>C41, C42</t>
   </si>
   <si>
-    <t>X2, X5</t>
-  </si>
-  <si>
     <t>C8, C10, C11, C23, C24</t>
   </si>
   <si>
@@ -575,9 +563,6 @@
     <t>IC3, IC9</t>
   </si>
   <si>
-    <t>IC2, IC4, IC5, IC6, IC11, IC12</t>
-  </si>
-  <si>
     <t>OEPS080017</t>
   </si>
   <si>
@@ -597,6 +582,21 @@
   </si>
   <si>
     <t>N.A.</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C7, C9, C12, C14, C16, C17, C18, C25, C26, C27, C19, C20, C21, C22,  C28, C29, C30, C31</t>
+  </si>
+  <si>
+    <t>X2, X5, X9</t>
+  </si>
+  <si>
+    <t>X4, X10</t>
+  </si>
+  <si>
+    <t>R2, R6, R8, R10, R11, R12, R13, R14, R17, R18, R19, R34</t>
+  </si>
+  <si>
+    <t>IC2, IC4, IC5, IC6, IC11, IC12, IC13, IC14, IC15, C16, IC17, IC18</t>
   </si>
 </sst>
 </file>
@@ -669,9 +669,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -691,7 +689,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -730,26 +730,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0E1B8A0-5F1C-47E2-B43A-1F1443A6183E}" name="Table_VestibularVR_H2_module_v1_1__3" displayName="Table_VestibularVR_H2_module_v1_1__3" ref="A5:H35" tableType="queryTable" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E0E1B8A0-5F1C-47E2-B43A-1F1443A6183E}" name="Table_VestibularVR_H2_module_v1_1__3" displayName="Table_VestibularVR_H2_module_v1_1__3" ref="A5:H35" tableType="queryTable" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A5:H35" xr:uid="{E0E1B8A0-5F1C-47E2-B43A-1F1443A6183E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D59A32E2-9654-4A4A-BB60-0299134151B3}" uniqueName="1" name="Qty" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{B4A92802-2CD7-4E87-98FF-4654F8487193}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{2E7BB510-1952-4C95-946C-91BEFBB2B314}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{CB596946-E4A7-46D7-AF8D-F591858DA85C}" uniqueName="9" name="OEPS" queryTableFieldId="9" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{BC43D583-64D1-4B91-9AEB-B3EEDEA134EC}" uniqueName="8" name="MPN" queryTableFieldId="8" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F179BED6-894F-406C-963E-3DDACA84842D}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D9BFE591-6B22-4BEB-9727-31AC27C32CE6}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{E4586192-6BE6-4B99-9622-BAD451E766D7}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{D59A32E2-9654-4A4A-BB60-0299134151B3}" uniqueName="1" name="Qty" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{B4A92802-2CD7-4E87-98FF-4654F8487193}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2E7BB510-1952-4C95-946C-91BEFBB2B314}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{CB596946-E4A7-46D7-AF8D-F591858DA85C}" uniqueName="9" name="OEPS" queryTableFieldId="9" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{BC43D583-64D1-4B91-9AEB-B3EEDEA134EC}" uniqueName="8" name="MPN" queryTableFieldId="8" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F179BED6-894F-406C-963E-3DDACA84842D}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D9BFE591-6B22-4BEB-9727-31AC27C32CE6}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E4586192-6BE6-4B99-9622-BAD451E766D7}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -787,7 +787,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -893,7 +893,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1035,7 +1035,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1045,36 +1045,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7E8E4E-AF52-4D1D-B285-902031C6AE83}">
   <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1100,12 +1100,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -1126,7 +1126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1152,12 +1152,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>19</v>
@@ -1178,7 +1178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -1204,12 +1204,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>105</v>
@@ -1230,7 +1230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1282,12 +1282,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>97</v>
@@ -1308,7 +1308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1334,12 +1334,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>130</v>
@@ -1360,7 +1360,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -1438,12 +1438,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>5</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>27</v>
@@ -1464,12 +1464,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>31</v>
@@ -1490,7 +1490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -1542,59 +1542,59 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="G23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>1</v>
       </c>
@@ -1620,12 +1620,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>69</v>
@@ -1646,7 +1646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>1</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1</v>
       </c>
@@ -1698,12 +1698,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>91</v>
@@ -1724,33 +1724,33 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>1</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>1</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>1</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>1</v>
       </c>
@@ -1854,12 +1854,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>65</v>
@@ -1880,7 +1880,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1890,7 +1890,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1900,14 +1900,14 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>